<commit_message>
tez yazimi icin deneyler
</commit_message>
<xml_diff>
--- a/belgeler/GANTT CHART.xlsx
+++ b/belgeler/GANTT CHART.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\behlul\Desktop\BitirmeProjesi\belgeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B0F015-BA2C-44AE-B296-A9BF1977BA15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F318827-E77F-4AAC-8E2E-DD2D69188740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
   <si>
     <t>Görev</t>
   </si>
@@ -78,16 +78,362 @@
   </si>
   <si>
     <t>Ms. Pac-Man oyununun araştırılması</t>
+  </si>
+  <si>
+    <t>Oyun sayısı</t>
+  </si>
+  <si>
+    <t>Ortalama</t>
+  </si>
+  <si>
+    <t>8574.75</t>
+  </si>
+  <si>
+    <t>Medyan</t>
+  </si>
+  <si>
+    <t>Standart sapma</t>
+  </si>
+  <si>
+    <t>4516.43</t>
+  </si>
+  <si>
+    <t>Standart hata</t>
+  </si>
+  <si>
+    <t>142.82</t>
+  </si>
+  <si>
+    <t>En düşük skor</t>
+  </si>
+  <si>
+    <t>En yüksek skor</t>
+  </si>
+  <si>
+    <t>StarterGhosts</t>
+  </si>
+  <si>
+    <t>Oyun Sırası</t>
+  </si>
+  <si>
+    <t>Oyun Skoru</t>
+  </si>
+  <si>
+    <t>Ortalama puan</t>
+  </si>
+  <si>
+    <t>5002.47</t>
+  </si>
+  <si>
+    <t>Standart Hata</t>
+  </si>
+  <si>
+    <t>1168.93</t>
+  </si>
+  <si>
+    <t>StarterGhostsComm</t>
+  </si>
+  <si>
+    <t>3062.71</t>
+  </si>
+  <si>
+    <t>96.85</t>
+  </si>
+  <si>
+    <t>1. Oyun</t>
+  </si>
+  <si>
+    <t>2. Oyun</t>
+  </si>
+  <si>
+    <t>3. Oyun</t>
+  </si>
+  <si>
+    <t>4. Oyun</t>
+  </si>
+  <si>
+    <t>5. Oyun</t>
+  </si>
+  <si>
+    <t>6. Oyun</t>
+  </si>
+  <si>
+    <t>7. Oyun</t>
+  </si>
+  <si>
+    <t>8. Oyun</t>
+  </si>
+  <si>
+    <t>9. Oyun</t>
+  </si>
+  <si>
+    <t>10. Oyun</t>
+  </si>
+  <si>
+    <t>Sonuçlar</t>
+  </si>
+  <si>
+    <t>4257.86</t>
+  </si>
+  <si>
+    <t>1346.45</t>
+  </si>
+  <si>
+    <t>StarterPacman</t>
+  </si>
+  <si>
+    <t>1107.65</t>
+  </si>
+  <si>
+    <t>35.02</t>
+  </si>
+  <si>
+    <t>1427.88</t>
+  </si>
+  <si>
+    <t>45.15</t>
+  </si>
+  <si>
+    <t>CIG 2017</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Average Score</t>
+  </si>
+  <si>
+    <t>SubtleBattle</t>
+  </si>
+  <si>
+    <t>10260.38</t>
+  </si>
+  <si>
+    <t>giangrocker</t>
+  </si>
+  <si>
+    <t>9147.60</t>
+  </si>
+  <si>
+    <t>thunder</t>
+  </si>
+  <si>
+    <t>8861.12</t>
+  </si>
+  <si>
+    <t>ToSc</t>
+  </si>
+  <si>
+    <t>8388.80</t>
+  </si>
+  <si>
+    <t>BaHe</t>
+  </si>
+  <si>
+    <t>8245.39</t>
+  </si>
+  <si>
+    <t>AlDo</t>
+  </si>
+  <si>
+    <t>8107.35</t>
+  </si>
+  <si>
+    <t>ArHe</t>
+  </si>
+  <si>
+    <t>7426.49</t>
+  </si>
+  <si>
+    <t>NiStTiTi</t>
+  </si>
+  <si>
+    <t>6798.07</t>
+  </si>
+  <si>
+    <t>ShMaRaSi</t>
+  </si>
+  <si>
+    <t>6633.92</t>
+  </si>
+  <si>
+    <t>imadhajjar</t>
+  </si>
+  <si>
+    <t>5646.26</t>
+  </si>
+  <si>
+    <t>CIG 2018</t>
+  </si>
+  <si>
+    <t>Squillyprice01</t>
+  </si>
+  <si>
+    <t>7736.63</t>
+  </si>
+  <si>
+    <t>GiangCao</t>
+  </si>
+  <si>
+    <t>7516.63</t>
+  </si>
+  <si>
+    <t>6733.13</t>
+  </si>
+  <si>
+    <t>PacMaas</t>
+  </si>
+  <si>
+    <t>Starter PacMan</t>
+  </si>
+  <si>
+    <t>5865.5</t>
+  </si>
+  <si>
+    <t>StarterPacManOneJunction</t>
+  </si>
+  <si>
+    <t>1134.25</t>
+  </si>
+  <si>
+    <t>StarterNNPacMan</t>
+  </si>
+  <si>
+    <t>user76</t>
+  </si>
+  <si>
+    <t>Sıralama</t>
+  </si>
+  <si>
+    <t>Takım Adları</t>
+  </si>
+  <si>
+    <t>Ortalama Skor</t>
+  </si>
+  <si>
+    <t>MaFr</t>
+  </si>
+  <si>
+    <t>2223.86</t>
+  </si>
+  <si>
+    <t>TiIsFePre</t>
+  </si>
+  <si>
+    <t>2853.79</t>
+  </si>
+  <si>
+    <t>3047.42</t>
+  </si>
+  <si>
+    <t>Starter Ghost Communicating</t>
+  </si>
+  <si>
+    <t>3243.27</t>
+  </si>
+  <si>
+    <t>3276.37</t>
+  </si>
+  <si>
+    <t>StScThSe</t>
+  </si>
+  <si>
+    <t>3299.46</t>
+  </si>
+  <si>
+    <t>3341.16</t>
+  </si>
+  <si>
+    <t>LeHoNiPo</t>
+  </si>
+  <si>
+    <t>3397.88</t>
+  </si>
+  <si>
+    <t>3415.34</t>
+  </si>
+  <si>
+    <t>DoWe</t>
+  </si>
+  <si>
+    <t>4167.21</t>
+  </si>
+  <si>
+    <t>AnAtVaTs</t>
+  </si>
+  <si>
+    <t>4443.13</t>
+  </si>
+  <si>
+    <t>Starter Ghost</t>
+  </si>
+  <si>
+    <t>4466.42</t>
+  </si>
+  <si>
+    <t>SaHo</t>
+  </si>
+  <si>
+    <t>4507.71</t>
+  </si>
+  <si>
+    <t>ImHa</t>
+  </si>
+  <si>
+    <t>6054.58</t>
+  </si>
+  <si>
+    <t>KeAlAnPe</t>
+  </si>
+  <si>
+    <t>6509.33</t>
+  </si>
+  <si>
+    <t>MaZeAnKu</t>
+  </si>
+  <si>
+    <t>6565.19</t>
+  </si>
+  <si>
+    <t>RiMu</t>
+  </si>
+  <si>
+    <t>6572.21</t>
+  </si>
+  <si>
+    <t>FlBe</t>
+  </si>
+  <si>
+    <t>10557.59</t>
+  </si>
+  <si>
+    <t>Oyuncu</t>
+  </si>
+  <si>
+    <t>3859.13</t>
+  </si>
+  <si>
+    <t>StarterGhost</t>
+  </si>
+  <si>
+    <t>4288.25</t>
+  </si>
+  <si>
+    <t>4864.81</t>
+  </si>
+  <si>
+    <t>4948.88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +471,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +515,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -174,14 +556,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyFill="0">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -192,8 +681,88 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Task" xfId="1" xr:uid="{64108E47-4BF5-432D-BE10-AFC437216E00}"/>
   </cellStyles>
@@ -1501,17 +2070,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,6 +2269,1171 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>43724</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="9">
+        <v>6043</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="8">
+        <v>7465</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="8">
+        <v>5265</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="8">
+        <v>820</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="8">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="8">
+        <v>32330</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="8">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="8">
+        <v>2940</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="8">
+        <v>12260</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="9">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="8">
+        <v>6010</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="8">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="8">
+        <v>6790</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="8">
+        <v>20510</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="8">
+        <v>6740</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="8">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="8">
+        <v>10330</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="8">
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="8">
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="8">
+        <v>13010</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="8">
+        <v>5420</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="10">
+        <f>AVERAGE(C52:C61)</f>
+        <v>8842</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="9">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="11">
+        <v>20510</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="8">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="11">
+        <v>2940</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="11">
+        <v>6765</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" s="8">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="11">
+        <v>1581</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="8">
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="8">
+        <v>1</v>
+      </c>
+      <c r="C71" s="8">
+        <v>8450</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="8">
+        <v>2</v>
+      </c>
+      <c r="C72" s="8">
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="8">
+        <v>3</v>
+      </c>
+      <c r="C73" s="8">
+        <v>9920</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="8">
+        <v>4</v>
+      </c>
+      <c r="C74" s="8">
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="8">
+        <v>5</v>
+      </c>
+      <c r="C75" s="8">
+        <v>8890</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="8">
+        <v>6</v>
+      </c>
+      <c r="C76" s="8">
+        <v>14880</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="8">
+        <v>7</v>
+      </c>
+      <c r="C77" s="8">
+        <v>15270</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="8">
+        <v>8</v>
+      </c>
+      <c r="C78" s="8">
+        <v>7380</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="8">
+        <v>9</v>
+      </c>
+      <c r="C79" s="8">
+        <v>10890</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="8">
+        <v>10</v>
+      </c>
+      <c r="C80" s="8">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" s="10">
+        <f>AVERAGE(C71:C80)</f>
+        <v>9406</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="11">
+        <v>15270</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="11">
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" s="11">
+        <v>9405</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="13">
+        <f>STDEV(C71:C80)</f>
+        <v>3896.4177280049316</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="8"/>
+      <c r="C89" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="20">
+        <v>6870</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="20">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" s="20">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="20">
+        <v>18270</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="20">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="20">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="20">
+        <v>10090</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="20">
+        <v>7540</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C98" s="20">
+        <v>7710</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="20">
+        <v>9070</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C100" s="21">
+        <f>AVERAGE(C90:C99)</f>
+        <v>7493</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" s="22">
+        <f>MAX(C90:C99)</f>
+        <v>18270</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="22">
+        <f>MIN(C90:C99)</f>
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" s="22">
+        <v>7205</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B109" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B110" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B111" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B112" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B113" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B114" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B115" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B116" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B117" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B118" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B119" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B121" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B122" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B123" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B124" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C124" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B125" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C125" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B126" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C126" s="19">
+        <v>6275</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B127" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C127" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="B128" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C128" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B129" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C129" s="19">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B130" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C130" s="19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B133" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C133" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D133" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B134" s="26">
+        <v>1</v>
+      </c>
+      <c r="C134" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D134" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B135" s="26">
+        <v>2</v>
+      </c>
+      <c r="C135" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D135" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B136" s="26">
+        <v>3</v>
+      </c>
+      <c r="C136" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B137" s="27"/>
+      <c r="C137" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D137" s="19">
+        <v>6275</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B138" s="26">
+        <v>4</v>
+      </c>
+      <c r="C138" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D138" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B139" s="26">
+        <v>5</v>
+      </c>
+      <c r="C139" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D139" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B140" s="26">
+        <v>6</v>
+      </c>
+      <c r="C140" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D140" s="19">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B141" s="26">
+        <v>7</v>
+      </c>
+      <c r="C141" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D141" s="19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="23"/>
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+    </row>
+    <row r="143" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="23"/>
+      <c r="C143" s="24"/>
+      <c r="D143" s="24"/>
+    </row>
+    <row r="144" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="23"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+    </row>
+    <row r="147" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B147" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C147" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D147" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B148" s="26">
+        <v>1</v>
+      </c>
+      <c r="C148" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D148" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B149" s="26">
+        <v>2</v>
+      </c>
+      <c r="C149" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D149" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="33">
+        <v>3</v>
+      </c>
+      <c r="C150" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D150" s="30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="35">
+        <v>4</v>
+      </c>
+      <c r="C151" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D151" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B152" s="34">
+        <v>5</v>
+      </c>
+      <c r="C152" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D152" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B153" s="26">
+        <v>6</v>
+      </c>
+      <c r="C153" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D153" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B154" s="26">
+        <v>7</v>
+      </c>
+      <c r="C154" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D154" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B155" s="26">
+        <v>8</v>
+      </c>
+      <c r="C155" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D155" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B156" s="26">
+        <v>9</v>
+      </c>
+      <c r="C156" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D156" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B157" s="26">
+        <v>10</v>
+      </c>
+      <c r="C157" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D157" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="33">
+        <v>11</v>
+      </c>
+      <c r="C158" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D158" s="30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="35">
+        <v>12</v>
+      </c>
+      <c r="C159" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D159" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B160" s="34">
+        <v>13</v>
+      </c>
+      <c r="C160" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D160" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B161" s="26">
+        <v>14</v>
+      </c>
+      <c r="C161" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D161" s="29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B162" s="26">
+        <v>15</v>
+      </c>
+      <c r="C162" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D162" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B163" s="26">
+        <v>16</v>
+      </c>
+      <c r="C163" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D163" s="29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B164" s="26">
+        <v>17</v>
+      </c>
+      <c r="C164" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D164" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B165" s="26">
+        <v>18</v>
+      </c>
+      <c r="C165" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D165" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B169" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C169" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D169" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B170" s="26">
+        <v>1</v>
+      </c>
+      <c r="C170" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D170" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B171" s="26">
+        <v>2</v>
+      </c>
+      <c r="C171" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D171" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B172" s="26">
+        <v>3</v>
+      </c>
+      <c r="C172" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D172" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B173" s="26">
+        <v>4</v>
+      </c>
+      <c r="C173" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D173" s="29" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iyilestirmeye calistim ama puanlar dustu xd
</commit_message>
<xml_diff>
--- a/belgeler/GANTT CHART.xlsx
+++ b/belgeler/GANTT CHART.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\behlul\Desktop\BitirmeProjesi\belgeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F318827-E77F-4AAC-8E2E-DD2D69188740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258BC785-C9C6-4AE3-B2BC-DBD8425E6AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="133">
   <si>
     <t>Görev</t>
   </si>
@@ -423,6 +423,15 @@
   </si>
   <si>
     <t>4948.88</t>
+  </si>
+  <si>
+    <t>Tasarlanan Ms. Pac-Man</t>
+  </si>
+  <si>
+    <t>Alıntı sayıları</t>
+  </si>
+  <si>
+    <t>Tahminler</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +509,35 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -670,7 +708,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,6 +797,36 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2070,16 +2138,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G173"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69:F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
@@ -2610,95 +2678,169 @@
         <v>9940</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E69" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" s="44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="8">
-        <v>1</v>
+      <c r="E70" s="45">
+        <v>12</v>
+      </c>
+      <c r="F70" s="46">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C71" s="8">
         <v>8450</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="8">
-        <v>2</v>
+      <c r="E71" s="45">
+        <v>7</v>
+      </c>
+      <c r="F71" s="46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C72" s="8">
         <v>10750</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="8">
-        <v>3</v>
+      <c r="E72" s="45">
+        <v>16</v>
+      </c>
+      <c r="F72" s="46">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C73" s="8">
         <v>9920</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="8">
-        <v>4</v>
+      <c r="E73" s="45">
+        <v>12</v>
+      </c>
+      <c r="F73" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C74" s="8">
         <v>3490</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="8">
-        <v>5</v>
+      <c r="E74" s="45">
+        <v>11</v>
+      </c>
+      <c r="F74" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C75" s="8">
         <v>8890</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="8">
-        <v>6</v>
+      <c r="E75" s="45">
+        <v>14</v>
+      </c>
+      <c r="F75" s="46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C76" s="8">
         <v>14880</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="8">
-        <v>7</v>
+      <c r="E76" s="45">
+        <v>11</v>
+      </c>
+      <c r="F76" s="46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C77" s="8">
         <v>15270</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="8">
-        <v>8</v>
+      <c r="E77" s="45">
+        <v>9</v>
+      </c>
+      <c r="F77" s="46">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C78" s="8">
         <v>7380</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="8">
-        <v>9</v>
+      <c r="E78" s="45">
+        <v>21</v>
+      </c>
+      <c r="F78" s="46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C79" s="8">
         <v>10890</v>
       </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="8">
-        <v>10</v>
+      <c r="E79" s="45">
+        <v>12</v>
+      </c>
+      <c r="F79" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C80" s="8">
         <v>4140</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E80" s="45">
+        <v>26</v>
+      </c>
+      <c r="F80" s="46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>28</v>
       </c>
@@ -2706,32 +2848,56 @@
         <f>AVERAGE(C71:C80)</f>
         <v>9406</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E81" s="45">
+        <v>21</v>
+      </c>
+      <c r="F81" s="46">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C82" s="11">
         <v>15270</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E82" s="45">
+        <v>26</v>
+      </c>
+      <c r="F82" s="46">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C83" s="11">
         <v>3490</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E83" s="45">
+        <v>17</v>
+      </c>
+      <c r="F83" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C84" s="11">
         <v>9405</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E84" s="45">
+        <v>9</v>
+      </c>
+      <c r="F84" s="46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
         <v>19</v>
       </c>
@@ -2739,51 +2905,101 @@
         <f>STDEV(C71:C80)</f>
         <v>3896.4177280049316</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E85" s="45">
+        <v>11</v>
+      </c>
+      <c r="F85" s="46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E86" s="45">
+        <v>3</v>
+      </c>
+      <c r="F86" s="46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E87" s="45">
+        <v>7</v>
+      </c>
+      <c r="F87" s="46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B88" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E88" s="45">
+        <v>7</v>
+      </c>
+      <c r="F88" s="46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E89" s="45">
+        <v>153</v>
+      </c>
+      <c r="F89" s="46">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C90" s="20">
         <v>6870</v>
       </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E90" s="45">
+        <v>15</v>
+      </c>
+      <c r="F90" s="46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C91" s="20">
         <v>3320</v>
       </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E91" s="45">
+        <v>9</v>
+      </c>
+      <c r="F91" s="46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C92" s="20">
         <v>4040</v>
       </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E92" s="45">
+        <v>24</v>
+      </c>
+      <c r="F92" s="46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
         <v>38</v>
       </c>
@@ -2791,7 +3007,7 @@
         <v>18270</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="s">
         <v>39</v>
       </c>
@@ -2799,7 +3015,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
         <v>40</v>
       </c>
@@ -2807,7 +3023,7 @@
         <v>4980</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="s">
         <v>41</v>
       </c>
@@ -2895,272 +3111,275 @@
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B109" s="16" t="s">
+    <row r="109" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B109" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="C109" s="38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B110" s="17" t="s">
+    <row r="110" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B110" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="17" t="s">
+      <c r="C110" s="39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B111" s="17" t="s">
+    <row r="111" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B111" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C111" s="17" t="s">
+      <c r="C111" s="39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="112" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B112" s="17" t="s">
+    <row r="112" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C112" s="17" t="s">
+      <c r="C112" s="40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B113" s="17" t="s">
+    <row r="113" spans="2:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C113" s="42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B114" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C114" s="41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B114" s="17" t="s">
+    <row r="115" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B115" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C115" s="39" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B115" s="17" t="s">
+    <row r="116" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B116" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C116" s="39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B116" s="17" t="s">
+    <row r="117" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B117" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C117" s="39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B117" s="17" t="s">
+    <row r="118" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B118" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C117" s="17" t="s">
+      <c r="C118" s="39" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B118" s="17" t="s">
+    <row r="119" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B119" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C119" s="39" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B119" s="17" t="s">
+    <row r="120" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B120" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C119" s="17" t="s">
+      <c r="C120" s="39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="121" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B121" s="18" t="s">
+    <row r="122" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B122" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B122" s="16" t="s">
+    <row r="123" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B123" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C123" s="16" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B123" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C123" s="19" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B124" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B125" s="17" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B126" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C126" s="19">
-        <v>6275</v>
+        <v>60</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B127" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="19">
+        <v>6275</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B128" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C127" s="19" t="s">
+      <c r="C128" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="128" spans="2:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="B128" s="17" t="s">
+    <row r="129" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B129" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C128" s="19" t="s">
+      <c r="C129" s="19" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B129" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C129" s="19">
-        <v>535</v>
       </c>
     </row>
     <row r="130" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B130" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C130" s="19">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B131" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C130" s="19">
+      <c r="C131" s="19">
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B133" s="25" t="s">
+    <row r="134" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B134" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C133" s="25" t="s">
+      <c r="C134" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D133" s="25" t="s">
+      <c r="D134" s="25" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B134" s="26">
-        <v>1</v>
-      </c>
-      <c r="C134" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D134" s="19" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="135" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B135" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="136" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B136" s="26">
+        <v>2</v>
+      </c>
+      <c r="C136" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B137" s="26">
         <v>3</v>
       </c>
-      <c r="C136" s="19" t="s">
+      <c r="C137" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D136" s="19" t="s">
+      <c r="D137" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="137" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B137" s="27"/>
-      <c r="C137" s="19" t="s">
+    <row r="138" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B138" s="27"/>
+      <c r="C138" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D137" s="19">
+      <c r="D138" s="19">
         <v>6275</v>
       </c>
     </row>
-    <row r="138" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B138" s="26">
+    <row r="139" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B139" s="26">
         <v>4</v>
       </c>
-      <c r="C138" s="19" t="s">
+      <c r="C139" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D138" s="19" t="s">
+      <c r="D139" s="19" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="139" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B139" s="26">
-        <v>5</v>
-      </c>
-      <c r="C139" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D139" s="19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B140" s="26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D140" s="19">
-        <v>535</v>
+        <v>85</v>
+      </c>
+      <c r="D140" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="141" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B141" s="26">
+        <v>6</v>
+      </c>
+      <c r="C141" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D141" s="19">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B142" s="26">
         <v>7</v>
       </c>
-      <c r="C141" s="19" t="s">
+      <c r="C142" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D141" s="19">
+      <c r="D142" s="19">
         <v>120</v>
       </c>
-    </row>
-    <row r="142" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="23"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="24"/>
     </row>
     <row r="143" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="23"/>
@@ -3172,267 +3391,272 @@
       <c r="C144" s="24"/>
       <c r="D144" s="24"/>
     </row>
-    <row r="147" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B147" s="25" t="s">
+    <row r="145" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B145" s="23"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+    </row>
+    <row r="148" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B148" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C147" s="28" t="s">
+      <c r="C148" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D147" s="28" t="s">
+      <c r="D148" s="28" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B148" s="26">
-        <v>1</v>
-      </c>
-      <c r="C148" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D148" s="29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="149" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B149" s="26">
+        <v>1</v>
+      </c>
+      <c r="C149" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D149" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B150" s="26">
         <v>2</v>
       </c>
-      <c r="C149" s="29" t="s">
+      <c r="C150" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D149" s="29" t="s">
+      <c r="D150" s="29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="150" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="33">
+    <row r="151" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="33">
         <v>3</v>
       </c>
-      <c r="C150" s="30" t="s">
+      <c r="C151" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D150" s="30" t="s">
+      <c r="D151" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="35">
+    <row r="152" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="35">
         <v>4</v>
       </c>
-      <c r="C151" s="36" t="s">
+      <c r="C152" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D151" s="32" t="s">
+      <c r="D152" s="32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="152" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B152" s="34">
+    <row r="153" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B153" s="34">
         <v>5</v>
       </c>
-      <c r="C152" s="31" t="s">
+      <c r="C153" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D152" s="31" t="s">
+      <c r="D153" s="31" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B153" s="26">
-        <v>6</v>
-      </c>
-      <c r="C153" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D153" s="29" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="154" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B154" s="26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C154" s="29" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="155" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B155" s="26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C155" s="29" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="156" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B156" s="26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C156" s="29" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="157" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B157" s="26">
+        <v>9</v>
+      </c>
+      <c r="C157" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D157" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B158" s="26">
         <v>10</v>
       </c>
-      <c r="C157" s="29" t="s">
+      <c r="C158" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D157" s="29" t="s">
+      <c r="D158" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="158" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="33">
+    <row r="159" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="33">
         <v>11</v>
       </c>
-      <c r="C158" s="30" t="s">
+      <c r="C159" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D158" s="30" t="s">
+      <c r="D159" s="30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="159" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="35">
+    <row r="160" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="35">
         <v>12</v>
       </c>
-      <c r="C159" s="36" t="s">
+      <c r="C160" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D159" s="32" t="s">
+      <c r="D160" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="160" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B160" s="34">
+    <row r="161" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B161" s="34">
         <v>13</v>
       </c>
-      <c r="C160" s="31" t="s">
+      <c r="C161" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D160" s="31" t="s">
+      <c r="D161" s="31" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B161" s="26">
-        <v>14</v>
-      </c>
-      <c r="C161" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="D161" s="29" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="162" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B162" s="26">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C162" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D162" s="29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B163" s="26">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C163" s="29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D163" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="164" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B164" s="26">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C164" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D164" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="165" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B165" s="26">
+        <v>17</v>
+      </c>
+      <c r="C165" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D165" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B166" s="26">
         <v>18</v>
       </c>
-      <c r="C165" s="29" t="s">
+      <c r="C166" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D165" s="29" t="s">
+      <c r="D166" s="29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="169" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B169" s="25" t="s">
+    <row r="170" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B170" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C169" s="28" t="s">
+      <c r="C170" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D169" s="28" t="s">
+      <c r="D170" s="28" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B170" s="26">
-        <v>1</v>
-      </c>
-      <c r="C170" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D170" s="29" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="171" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B171" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C171" s="29" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="D171" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="172" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B172" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172" s="29" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="D172" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="173" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B173" s="26">
+        <v>3</v>
+      </c>
+      <c r="C173" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D173" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B174" s="26">
         <v>4</v>
       </c>
-      <c r="C173" s="29" t="s">
+      <c r="C174" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="D173" s="29" t="s">
+      <c r="D174" s="29" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>